<commit_message>
feat: Improve phone number validation in start scene
This commit improves the phone number validation in the start scene by adding a regular expression check for Uzbek phone numbers. It ensures that the phone number entered by the user matches the expected format, which is +998 followed by 9 digits. If the phone number is not in the correct format, an error message is displayed, prompting the user to enter the phone number again. This enhancement improves the user experience and prevents incorrect phone numbers from being stored in the system.
</commit_message>
<xml_diff>
--- a/src/data/test3.xlsx
+++ b/src/data/test3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="34">
   <si>
     <t>Номи</t>
   </si>
@@ -37,82 +37,76 @@
     <t>12 месяц</t>
   </si>
   <si>
-    <t>S24 Ultra</t>
+    <t xml:space="preserve">13C </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4/128gb  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">blue </t>
+  </si>
+  <si>
+    <t xml:space="preserve">black </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6/128gb  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">blue  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/256gb  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redmi 12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4/128gb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue </t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6/128gb </t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/256gb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note 13 </t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8/128gb </t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note 13Pro </t>
+  </si>
+  <si>
+    <t>Purple</t>
   </si>
   <si>
     <t xml:space="preserve">12/512gb </t>
   </si>
   <si>
-    <t xml:space="preserve">Titanium Gray </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Titanium Black </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Titanium Violet </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Titanium Yellow </t>
-  </si>
-  <si>
-    <t xml:space="preserve">12/256gb </t>
-  </si>
-  <si>
-    <t xml:space="preserve">S24+ </t>
-  </si>
-  <si>
-    <t>12/256gb </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Black </t>
-  </si>
-  <si>
-    <t xml:space="preserve">S24 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8/256gb </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gray </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8/128gb </t>
-  </si>
-  <si>
-    <t>S23 Ultra</t>
-  </si>
-  <si>
     <t xml:space="preserve">Green </t>
   </si>
   <si>
-    <t xml:space="preserve">Cream </t>
-  </si>
-  <si>
-    <t>S23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S23 </t>
-  </si>
-  <si>
-    <t>Z Fold 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blue </t>
-  </si>
-  <si>
-    <t>Z Flip 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8/512gb </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mint </t>
-  </si>
-  <si>
-    <t>Z Fold 4</t>
-  </si>
-  <si>
-    <t>S22</t>
+    <t xml:space="preserve">Note 13Pro + </t>
   </si>
   <si>
     <t xml:space="preserve">8/256gb 5G </t>
@@ -121,55 +115,7 @@
     <t xml:space="preserve">White </t>
   </si>
   <si>
-    <t xml:space="preserve">8/128gb 5G </t>
-  </si>
-  <si>
-    <t>A55</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Violet</t>
-  </si>
-  <si>
-    <t>Lime</t>
-  </si>
-  <si>
-    <t>A35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silver </t>
-  </si>
-  <si>
-    <t>A25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6/128gb </t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>Silver</t>
-  </si>
-  <si>
-    <t>A15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yellow </t>
-  </si>
-  <si>
-    <t>A05s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">black </t>
-  </si>
-  <si>
-    <t xml:space="preserve">green </t>
-  </si>
-  <si>
-    <t xml:space="preserve">silver </t>
+    <t xml:space="preserve">12/512gb 5G </t>
   </si>
 </sst>
 </file>
@@ -177,11 +123,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0\ [$UZS]_-;\-* #,##0\ [$UZS]_-;_-* &quot;-&quot;??\ [$UZS]_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0\ [$UZS]_-;\-* #,##0\ [$UZS]_-;_-* &quot;-&quot;??\ [$UZS]_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00\ &quot;₽&quot;_-;\-* #,##0.00\ &quot;₽&quot;_-;_-* &quot;-&quot;??\ &quot;₽&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -220,14 +166,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -240,6 +178,22 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -258,6 +212,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -266,7 +243,44 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -282,9 +296,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -293,74 +307,6 @@
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -385,7 +331,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -397,85 +409,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -493,7 +427,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -505,43 +475,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -553,13 +487,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -656,32 +602,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -694,8 +614,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -715,6 +650,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -729,158 +684,149 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -891,9 +837,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="27" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -921,7 +867,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="6" xfId="27" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="6" xfId="27" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1249,7 +1195,7 @@
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:G56"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -1296,16 +1242,16 @@
         <v>9</v>
       </c>
       <c r="D2" s="2">
-        <v>1140</v>
+        <v>138</v>
       </c>
       <c r="E2" s="2">
-        <v>1458</v>
+        <v>162</v>
       </c>
       <c r="F2" s="8">
-        <v>3888570</v>
+        <v>431970</v>
       </c>
       <c r="G2" s="8">
-        <v>2237470.83333333</v>
+        <v>248554.166666667</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1319,16 +1265,16 @@
         <v>10</v>
       </c>
       <c r="D3" s="2">
-        <v>1140</v>
+        <v>138</v>
       </c>
       <c r="E3" s="2">
-        <v>1458</v>
+        <v>162</v>
       </c>
       <c r="F3" s="8">
-        <v>3888570</v>
+        <v>431970</v>
       </c>
       <c r="G3" s="8">
-        <v>2237470.83333333</v>
+        <v>248554.166666667</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1336,22 +1282,22 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2">
-        <v>1140</v>
+        <v>146</v>
       </c>
       <c r="E4" s="2">
-        <v>1458</v>
+        <v>172.8</v>
       </c>
       <c r="F4" s="8">
-        <v>3888570</v>
+        <v>460950</v>
       </c>
       <c r="G4" s="8">
-        <v>2237470.83333333</v>
+        <v>265229.166666667</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1359,22 +1305,22 @@
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2">
-        <v>1140</v>
+        <v>146</v>
       </c>
       <c r="E5" s="2">
-        <v>1458</v>
+        <v>172.8</v>
       </c>
       <c r="F5" s="8">
-        <v>3888570</v>
+        <v>460950</v>
       </c>
       <c r="G5" s="8">
-        <v>2237470.83333333</v>
+        <v>265229.166666667</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1385,42 +1331,42 @@
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2">
-        <v>1070</v>
+        <v>155</v>
       </c>
       <c r="E6" s="2">
-        <v>1363.5</v>
+        <v>184.95</v>
       </c>
       <c r="F6" s="8">
-        <v>3636360</v>
+        <v>493290</v>
       </c>
       <c r="G6" s="8">
-        <v>2092350</v>
+        <v>283837.5</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2">
-        <v>1070</v>
+        <v>158</v>
       </c>
       <c r="E7" s="2">
-        <v>1363.5</v>
+        <v>189</v>
       </c>
       <c r="F7" s="8">
-        <v>3636360</v>
+        <v>504000</v>
       </c>
       <c r="G7" s="8">
-        <v>2092350</v>
+        <v>290000</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1431,318 +1377,318 @@
         <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8" s="2">
-        <v>850</v>
+        <v>158</v>
       </c>
       <c r="E8" s="2">
-        <v>1093.5</v>
+        <v>189</v>
       </c>
       <c r="F8" s="8">
-        <v>2916270</v>
+        <v>504000</v>
       </c>
       <c r="G8" s="8">
-        <v>1678012.5</v>
+        <v>290000</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D9" s="2">
-        <v>750</v>
+        <v>158</v>
       </c>
       <c r="E9" s="2">
-        <v>958.5</v>
+        <v>189</v>
       </c>
       <c r="F9" s="8">
-        <v>2556330</v>
+        <v>504000</v>
       </c>
       <c r="G9" s="8">
-        <v>1470904.16666667</v>
+        <v>290000</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2">
-        <v>750</v>
+        <v>163</v>
       </c>
       <c r="E10" s="2">
-        <v>958.5</v>
+        <v>195.75</v>
       </c>
       <c r="F10" s="8">
-        <v>2556330</v>
+        <v>522060</v>
       </c>
       <c r="G10" s="8">
-        <v>1470904.16666667</v>
+        <v>300391.666666667</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D11" s="2">
-        <v>710</v>
+        <v>163</v>
       </c>
       <c r="E11" s="2">
-        <v>904.5</v>
+        <v>195.75</v>
       </c>
       <c r="F11" s="8">
-        <v>2412270</v>
+        <v>522060</v>
       </c>
       <c r="G11" s="8">
-        <v>1388012.5</v>
+        <v>300391.666666667</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D12" s="2">
-        <v>980</v>
+        <v>163</v>
       </c>
       <c r="E12" s="2">
-        <v>1255.5</v>
+        <v>195.75</v>
       </c>
       <c r="F12" s="8">
-        <v>3348450</v>
+        <v>522060</v>
       </c>
       <c r="G12" s="8">
-        <v>1926687.5</v>
+        <v>300391.666666667</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D13" s="2">
-        <v>980</v>
+        <v>178</v>
       </c>
       <c r="E13" s="2">
-        <v>1255.5</v>
+        <v>216</v>
       </c>
       <c r="F13" s="8">
-        <v>3348450</v>
+        <v>576030</v>
       </c>
       <c r="G13" s="8">
-        <v>1926687.5</v>
+        <v>331445.833333333</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D14" s="2">
-        <v>980</v>
+        <v>193</v>
       </c>
       <c r="E14" s="2">
-        <v>1255.5</v>
+        <v>236.25</v>
       </c>
       <c r="F14" s="8">
-        <v>3348450</v>
+        <v>630000</v>
       </c>
       <c r="G14" s="8">
-        <v>1926687.5</v>
+        <v>362500</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D15" s="2">
-        <v>850</v>
+        <v>193</v>
       </c>
       <c r="E15" s="2">
-        <v>1093.5</v>
+        <v>236.25</v>
       </c>
       <c r="F15" s="8">
-        <v>2916270</v>
+        <v>630000</v>
       </c>
       <c r="G15" s="8">
-        <v>1678012.5</v>
+        <v>362500</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D16" s="2">
-        <v>850</v>
+        <v>193</v>
       </c>
       <c r="E16" s="2">
-        <v>1093.5</v>
+        <v>236.25</v>
       </c>
       <c r="F16" s="8">
-        <v>2916270</v>
+        <v>630000</v>
       </c>
       <c r="G16" s="8">
-        <v>1678012.5</v>
+        <v>362500</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D17" s="2">
-        <v>850</v>
+        <v>203</v>
       </c>
       <c r="E17" s="2">
-        <v>1093.5</v>
+        <v>249.75</v>
       </c>
       <c r="F17" s="8">
-        <v>2916270</v>
+        <v>666120</v>
       </c>
       <c r="G17" s="8">
-        <v>1678012.5</v>
+        <v>383283.333333333</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D18" s="2">
-        <v>660</v>
+        <v>213</v>
       </c>
       <c r="E18" s="2">
-        <v>837</v>
+        <v>263.25</v>
       </c>
       <c r="F18" s="8">
-        <v>2232300</v>
+        <v>702030</v>
       </c>
       <c r="G18" s="8">
-        <v>1284458.33333333</v>
+        <v>403945.833333333</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D19" s="2">
-        <v>660</v>
+        <v>213</v>
       </c>
       <c r="E19" s="2">
-        <v>837</v>
+        <v>263.25</v>
       </c>
       <c r="F19" s="8">
-        <v>2232300</v>
+        <v>702030</v>
       </c>
       <c r="G19" s="8">
-        <v>1284458.33333333</v>
+        <v>403945.833333333</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D20" s="2">
-        <v>625</v>
+        <v>213</v>
       </c>
       <c r="E20" s="2">
-        <v>789.75</v>
+        <v>263.25</v>
       </c>
       <c r="F20" s="8">
-        <v>2106300</v>
+        <v>702030</v>
       </c>
       <c r="G20" s="8">
-        <v>1211958.33333333</v>
+        <v>403945.833333333</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D21" s="2">
-        <v>625</v>
+        <v>268</v>
       </c>
       <c r="E21" s="2">
-        <v>789.75</v>
+        <v>337.5</v>
       </c>
       <c r="F21" s="8">
-        <v>2106300</v>
+        <v>900060</v>
       </c>
       <c r="G21" s="8">
-        <v>1211958.33333333</v>
+        <v>517891.666666667</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1750,22 +1696,22 @@
         <v>26</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D22" s="2">
-        <v>1210</v>
+        <v>268</v>
       </c>
       <c r="E22" s="2">
-        <v>1552.5</v>
+        <v>337.5</v>
       </c>
       <c r="F22" s="8">
-        <v>4140570</v>
+        <v>900060</v>
       </c>
       <c r="G22" s="8">
-        <v>2382470.83333333</v>
+        <v>517891.666666667</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1773,22 +1719,22 @@
         <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D23" s="2">
-        <v>1210</v>
+        <v>268</v>
       </c>
       <c r="E23" s="2">
-        <v>1552.5</v>
+        <v>337.5</v>
       </c>
       <c r="F23" s="8">
-        <v>4140570</v>
+        <v>900060</v>
       </c>
       <c r="G23" s="8">
-        <v>2382470.83333333</v>
+        <v>517891.666666667</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1796,22 +1742,22 @@
         <v>26</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D24" s="2">
-        <v>1210</v>
+        <v>323</v>
       </c>
       <c r="E24" s="2">
-        <v>1552.5</v>
+        <v>411.75</v>
       </c>
       <c r="F24" s="8">
-        <v>4140570</v>
+        <v>1098090</v>
       </c>
       <c r="G24" s="8">
-        <v>2382470.83333333</v>
+        <v>631837.5</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1819,736 +1765,386 @@
         <v>26</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D25" s="2">
-        <v>1160</v>
+        <v>323</v>
       </c>
       <c r="E25" s="2">
-        <v>1485</v>
+        <v>411.75</v>
       </c>
       <c r="F25" s="8">
-        <v>3960600</v>
+        <v>1098090</v>
       </c>
       <c r="G25" s="8">
-        <v>2278916.66666667</v>
+        <v>631837.5</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D26" s="2">
-        <v>1160</v>
+        <v>393</v>
       </c>
       <c r="E26" s="2">
-        <v>1485</v>
+        <v>506.25</v>
       </c>
       <c r="F26" s="8">
-        <v>3960600</v>
+        <v>1350090</v>
       </c>
       <c r="G26" s="8">
-        <v>2278916.66666667</v>
+        <v>776837.5</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D27" s="2">
-        <v>720</v>
+        <v>397</v>
       </c>
       <c r="E27" s="2">
-        <v>918</v>
+        <v>511.65</v>
       </c>
       <c r="F27" s="8">
-        <v>2448390</v>
+        <v>1364580</v>
       </c>
       <c r="G27" s="8">
-        <v>1408795.83333333</v>
+        <v>785175</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D28" s="2">
-        <v>690</v>
+        <v>397</v>
       </c>
       <c r="E28" s="2">
-        <v>877.5</v>
+        <v>511.65</v>
       </c>
       <c r="F28" s="8">
-        <v>2340240</v>
+        <v>1364580</v>
       </c>
       <c r="G28" s="8">
-        <v>1346566.66666667</v>
+        <v>785175</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D29" s="2">
-        <v>690</v>
+        <v>450</v>
       </c>
       <c r="E29" s="2">
-        <v>877.5</v>
+        <v>583.2</v>
       </c>
       <c r="F29" s="8">
-        <v>2340240</v>
+        <v>1555470</v>
       </c>
       <c r="G29" s="8">
-        <v>1346566.66666667</v>
+        <v>895012.5</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D30" s="2">
-        <v>1040</v>
+        <v>450</v>
       </c>
       <c r="E30" s="2">
-        <v>1336.5</v>
+        <v>583.2</v>
       </c>
       <c r="F30" s="8">
-        <v>3564540</v>
+        <v>1555470</v>
       </c>
       <c r="G30" s="8">
-        <v>2051025</v>
+        <v>895012.5</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D31" s="2">
-        <v>540</v>
+        <v>450</v>
       </c>
       <c r="E31" s="2">
-        <v>675</v>
+        <v>583.2</v>
       </c>
       <c r="F31" s="8">
-        <v>1800330</v>
+        <v>1555470</v>
       </c>
       <c r="G31" s="8">
-        <v>1035904.16666667</v>
+        <v>895012.5</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" s="2">
-        <v>540</v>
-      </c>
-      <c r="E32" s="2">
-        <v>675</v>
-      </c>
-      <c r="F32" s="8">
-        <v>1800330</v>
-      </c>
-      <c r="G32" s="8">
-        <v>1035904.16666667</v>
-      </c>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="2">
-        <v>490</v>
-      </c>
-      <c r="E33" s="2">
-        <v>607.5</v>
-      </c>
-      <c r="F33" s="8">
-        <v>1620150</v>
-      </c>
-      <c r="G33" s="8">
-        <v>932229.166666667</v>
-      </c>
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="2">
-        <v>490</v>
-      </c>
-      <c r="E34" s="2">
-        <v>607.5</v>
-      </c>
-      <c r="F34" s="8">
-        <v>1620150</v>
-      </c>
-      <c r="G34" s="8">
-        <v>932229.166666667</v>
-      </c>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" s="2">
-        <v>373</v>
-      </c>
-      <c r="E35" s="2">
-        <v>479.25</v>
-      </c>
-      <c r="F35" s="8">
-        <v>1278060</v>
-      </c>
-      <c r="G35" s="8">
-        <v>735391.666666667</v>
-      </c>
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D36" s="2">
-        <v>373</v>
-      </c>
-      <c r="E36" s="2">
-        <v>479.25</v>
-      </c>
-      <c r="F36" s="8">
-        <v>1278060</v>
-      </c>
-      <c r="G36" s="8">
-        <v>735391.666666667</v>
-      </c>
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="2">
-        <v>373</v>
-      </c>
-      <c r="E37" s="2">
-        <v>479.25</v>
-      </c>
-      <c r="F37" s="8">
-        <v>1278060</v>
-      </c>
-      <c r="G37" s="8">
-        <v>735391.666666667</v>
-      </c>
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="2">
-        <v>343</v>
-      </c>
-      <c r="E38" s="2">
-        <v>438.75</v>
-      </c>
-      <c r="F38" s="8">
-        <v>1170120</v>
-      </c>
-      <c r="G38" s="8">
-        <v>673283.333333333</v>
-      </c>
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D39" s="2">
-        <v>343</v>
-      </c>
-      <c r="E39" s="2">
-        <v>438.75</v>
-      </c>
-      <c r="F39" s="8">
-        <v>1170120</v>
-      </c>
-      <c r="G39" s="8">
-        <v>673283.333333333</v>
-      </c>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D40" s="2">
-        <v>332</v>
-      </c>
-      <c r="E40" s="2">
-        <v>423.9</v>
-      </c>
-      <c r="F40" s="8">
-        <v>1130640</v>
-      </c>
-      <c r="G40" s="8">
-        <v>650566.666666667</v>
-      </c>
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D41" s="2">
-        <v>332</v>
-      </c>
-      <c r="E41" s="2">
-        <v>423.9</v>
-      </c>
-      <c r="F41" s="8">
-        <v>1130640</v>
-      </c>
-      <c r="G41" s="8">
-        <v>650566.666666667</v>
-      </c>
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D42" s="2">
-        <v>332</v>
-      </c>
-      <c r="E42" s="2">
-        <v>423.9</v>
-      </c>
-      <c r="F42" s="8">
-        <v>1130640</v>
-      </c>
-      <c r="G42" s="8">
-        <v>650566.666666667</v>
-      </c>
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D43" s="2">
-        <v>332</v>
-      </c>
-      <c r="E43" s="2">
-        <v>423.9</v>
-      </c>
-      <c r="F43" s="8">
-        <v>1130640</v>
-      </c>
-      <c r="G43" s="8">
-        <v>650566.666666667</v>
-      </c>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D44" s="2">
-        <v>303</v>
-      </c>
-      <c r="E44" s="2">
-        <v>384.75</v>
-      </c>
-      <c r="F44" s="8">
-        <v>1026060</v>
-      </c>
-      <c r="G44" s="8">
-        <v>590391.666666667</v>
-      </c>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" s="2">
-        <v>303</v>
-      </c>
-      <c r="E45" s="2">
-        <v>384.75</v>
-      </c>
-      <c r="F45" s="8">
-        <v>1026060</v>
-      </c>
-      <c r="G45" s="8">
-        <v>590391.666666667</v>
-      </c>
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
     </row>
     <row r="46" spans="1:7">
-      <c r="A46" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D46" s="2">
-        <v>228</v>
-      </c>
-      <c r="E46" s="2">
-        <v>283.5</v>
-      </c>
-      <c r="F46" s="8">
-        <v>756000</v>
-      </c>
-      <c r="G46" s="8">
-        <v>435000</v>
-      </c>
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D47" s="2">
-        <v>228</v>
-      </c>
-      <c r="E47" s="2">
-        <v>283.5</v>
-      </c>
-      <c r="F47" s="8">
-        <v>756000</v>
-      </c>
-      <c r="G47" s="8">
-        <v>435000</v>
-      </c>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D48" s="2">
-        <v>228</v>
-      </c>
-      <c r="E48" s="2">
-        <v>283.5</v>
-      </c>
-      <c r="F48" s="8">
-        <v>756000</v>
-      </c>
-      <c r="G48" s="8">
-        <v>435000</v>
-      </c>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D49" s="2">
-        <v>160</v>
-      </c>
-      <c r="E49" s="2">
-        <v>191.7</v>
-      </c>
-      <c r="F49" s="8">
-        <v>511350</v>
-      </c>
-      <c r="G49" s="8">
-        <v>294229.166666667</v>
-      </c>
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D50" s="2">
-        <v>160</v>
-      </c>
-      <c r="E50" s="2">
-        <v>191.7</v>
-      </c>
-      <c r="F50" s="8">
-        <v>511350</v>
-      </c>
-      <c r="G50" s="8">
-        <v>294229.166666667</v>
-      </c>
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
     </row>
     <row r="51" spans="1:7">
-      <c r="A51" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51" s="2">
-        <v>188</v>
-      </c>
-      <c r="E51" s="2">
-        <v>229.5</v>
-      </c>
-      <c r="F51" s="8">
-        <v>612150</v>
-      </c>
-      <c r="G51" s="8">
-        <v>352229.166666667</v>
-      </c>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
     </row>
     <row r="52" spans="1:7">
-      <c r="A52" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D52" s="2">
-        <v>188</v>
-      </c>
-      <c r="E52" s="2">
-        <v>229.5</v>
-      </c>
-      <c r="F52" s="8">
-        <v>612150</v>
-      </c>
-      <c r="G52" s="8">
-        <v>352229.166666667</v>
-      </c>
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
     </row>
     <row r="53" spans="1:7">
-      <c r="A53" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D53" s="2">
-        <v>188</v>
-      </c>
-      <c r="E53" s="2">
-        <v>229.5</v>
-      </c>
-      <c r="F53" s="8">
-        <v>612150</v>
-      </c>
-      <c r="G53" s="8">
-        <v>352229.166666667</v>
-      </c>
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
     </row>
     <row r="54" spans="1:7">
-      <c r="A54" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D54" s="2">
-        <v>147</v>
-      </c>
-      <c r="E54" s="2">
-        <v>174.15</v>
-      </c>
-      <c r="F54" s="8">
-        <v>464520</v>
-      </c>
-      <c r="G54" s="8">
-        <v>267283.333333333</v>
-      </c>
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D55" s="2">
-        <v>147</v>
-      </c>
-      <c r="E55" s="2">
-        <v>174.15</v>
-      </c>
-      <c r="F55" s="8">
-        <v>464520</v>
-      </c>
-      <c r="G55" s="8">
-        <v>267283.333333333</v>
-      </c>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D56" s="2">
-        <v>147</v>
-      </c>
-      <c r="E56" s="2">
-        <v>174.15</v>
-      </c>
-      <c r="F56" s="8">
-        <v>464520</v>
-      </c>
-      <c r="G56" s="8">
-        <v>267283.333333333</v>
-      </c>
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" s="3"/>

</xml_diff>